<commit_message>
Worked more on fault analysis
</commit_message>
<xml_diff>
--- a/Fault Calcs.xlsx
+++ b/Fault Calcs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\my.files.iastate.edu\Users\kangeliu\EE457\ee457project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\EE457\ee457project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Bus Num</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Bus 4</t>
+  </si>
+  <si>
+    <t>I0</t>
+  </si>
+  <si>
+    <t>I+</t>
+  </si>
+  <si>
+    <t>I-</t>
+  </si>
+  <si>
+    <t>Angle</t>
   </si>
 </sst>
 </file>
@@ -390,7 +402,7 @@
   <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:H7"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +449,7 @@
         <v>-52.613900000000001</v>
       </c>
       <c r="D4">
-        <f>SQRT((B4)^2+(C4)^2)</f>
+        <f t="shared" ref="D4:D20" si="0">SQRT((B4)^2+(C4)^2)</f>
         <v>52.654963014135717</v>
       </c>
       <c r="F4">
@@ -462,7 +474,7 @@
         <v>-53.723199999999999</v>
       </c>
       <c r="D5">
-        <f>SQRT((B5)^2+(C5)^2)</f>
+        <f t="shared" si="0"/>
         <v>55.956414900259645</v>
       </c>
       <c r="F5">
@@ -472,7 +484,7 @@
         <v>-63.898000000000003</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H20" si="0">SQRT((F5)^2+(G5)^2)</f>
+        <f t="shared" ref="H5:H20" si="1">SQRT((F5)^2+(G5)^2)</f>
         <v>66.331107064182191</v>
       </c>
     </row>
@@ -487,7 +499,7 @@
         <v>-48.035499999999999</v>
       </c>
       <c r="D6">
-        <f>SQRT((B6)^2+(C6)^2)</f>
+        <f t="shared" si="0"/>
         <v>50.970170987549182</v>
       </c>
       <c r="F6">
@@ -497,7 +509,7 @@
         <v>-58.210999999999999</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61.353720128123449</v>
       </c>
     </row>
@@ -512,18 +524,18 @@
         <v>-20.9193</v>
       </c>
       <c r="D7">
-        <f>SQRT((B7)^2+(C7)^2)</f>
+        <f t="shared" si="0"/>
         <v>21.947817943704564</v>
       </c>
       <c r="F7">
-        <v>4.2830000000000004</v>
+        <v>3.9594999999999998</v>
       </c>
       <c r="G7">
-        <v>-15.3537</v>
+        <v>-13.8637</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
-        <v>15.939893120407049</v>
+        <f t="shared" si="1"/>
+        <v>14.418037936557109</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -537,18 +549,18 @@
         <v>-29.837900000000001</v>
       </c>
       <c r="D8">
-        <f>SQRT((B8)^2+(C8)^2)</f>
+        <f t="shared" si="0"/>
         <v>31.694783057310868</v>
       </c>
       <c r="F8">
-        <v>7.1260000000000003</v>
+        <v>6.6231999999999998</v>
       </c>
       <c r="G8">
-        <v>-22.672000000000001</v>
+        <v>-20.9344</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
-        <v>23.765509883021654</v>
+        <f t="shared" si="1"/>
+        <v>21.957137372617588</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -562,18 +574,18 @@
         <v>-20.553599999999999</v>
       </c>
       <c r="D9">
-        <f>SQRT((B9)^2+(C9)^2)</f>
+        <f t="shared" si="0"/>
         <v>22.016606918415018</v>
       </c>
       <c r="F9">
-        <v>5.1083999999999996</v>
+        <v>4.9508000000000001</v>
       </c>
       <c r="G9">
-        <v>-14.4184</v>
+        <v>-14.007199999999999</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
-        <v>15.296601227723759</v>
+        <f t="shared" si="1"/>
+        <v>14.856381540604024</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -587,18 +599,18 @@
         <v>-22.391400000000001</v>
       </c>
       <c r="D10">
-        <f>SQRT((B10)^2+(C10)^2)</f>
+        <f t="shared" si="0"/>
         <v>23.887768519683878</v>
       </c>
       <c r="F10">
-        <v>5.5152000000000001</v>
+        <v>5.0475000000000003</v>
       </c>
       <c r="G10">
-        <v>-16.927</v>
+        <v>-15.167</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>17.802830113215144</v>
+        <f t="shared" si="1"/>
+        <v>15.984841108062351</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -612,18 +624,18 @@
         <v>-23.030999999999999</v>
       </c>
       <c r="D11">
-        <f>SQRT((B11)^2+(C11)^2)</f>
+        <f t="shared" si="0"/>
         <v>24.559431684996294</v>
       </c>
       <c r="F11">
-        <v>5.6158000000000001</v>
+        <v>5.4569999999999999</v>
       </c>
       <c r="G11">
-        <v>-16.087199999999999</v>
+        <v>-15.664</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
-        <v>17.039225730061798</v>
+        <f t="shared" si="1"/>
+        <v>16.58733688691467</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -637,18 +649,18 @@
         <v>-18.940999999999999</v>
       </c>
       <c r="D12">
-        <f>SQRT((B12)^2+(C12)^2)</f>
+        <f t="shared" si="0"/>
         <v>19.376288008800859</v>
       </c>
       <c r="F12">
-        <v>2.9935</v>
+        <v>2.5451999999999999</v>
       </c>
       <c r="G12">
-        <v>-17.340599999999998</v>
+        <v>-12.442</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
-        <v>17.597086423894154</v>
+        <f t="shared" si="1"/>
+        <v>12.69966168998214</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -662,18 +674,18 @@
         <v>-3.3321000000000001</v>
       </c>
       <c r="D13">
-        <f>SQRT((B13)^2+(C13)^2)</f>
+        <f t="shared" si="0"/>
         <v>3.4533374306603752</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.58919999999999995</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>-2.343</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.4159481865304975</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -687,18 +699,18 @@
         <v>-26.456900000000001</v>
       </c>
       <c r="D14">
-        <f>SQRT((B14)^2+(C14)^2)</f>
+        <f t="shared" si="0"/>
         <v>27.602075197709322</v>
       </c>
       <c r="F14">
-        <v>5.2515000000000001</v>
+        <v>5.1891999999999996</v>
       </c>
       <c r="G14">
-        <v>-18.4892</v>
+        <v>-18.247900000000001</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
-        <v>19.220529880573011</v>
+        <f t="shared" si="1"/>
+        <v>18.971390329915202</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -712,18 +724,18 @@
         <v>-26.972799999999999</v>
       </c>
       <c r="D15">
-        <f>SQRT((B15)^2+(C15)^2)</f>
+        <f t="shared" si="0"/>
         <v>28.828579331628536</v>
       </c>
       <c r="F15">
-        <v>7.0849000000000002</v>
+        <v>6.9977999999999998</v>
       </c>
       <c r="G15">
-        <v>-19.184699999999999</v>
+        <v>-18.9666</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
-        <v>20.45112520376324</v>
+        <f t="shared" si="1"/>
+        <v>20.216357743174214</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -737,18 +749,18 @@
         <v>-3.0992999999999999</v>
       </c>
       <c r="D16">
-        <f>SQRT((B16)^2+(C16)^2)</f>
+        <f t="shared" si="0"/>
         <v>3.2591915224484738</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.60450000000000004</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>-2.1263999999999998</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.2106553801983697</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -762,18 +774,18 @@
         <v>-19.913699999999999</v>
       </c>
       <c r="D17">
-        <f>SQRT((B17)^2+(C17)^2)</f>
+        <f t="shared" si="0"/>
         <v>20.579894190690094</v>
       </c>
       <c r="F17">
-        <v>3.5828000000000002</v>
+        <v>3.5808</v>
       </c>
       <c r="G17">
-        <v>-13.546799999999999</v>
+        <v>-13.5433</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
-        <v>14.012574570006755</v>
+        <f t="shared" si="1"/>
+        <v>14.008679578389962</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -787,18 +799,18 @@
         <v>-18.785299999999999</v>
       </c>
       <c r="D18">
-        <f>SQRT((B18)^2+(C18)^2)</f>
+        <f t="shared" si="0"/>
         <v>20.055174521554278</v>
       </c>
       <c r="F18">
-        <v>5.6375000000000002</v>
+        <v>4.5118999999999998</v>
       </c>
       <c r="G18">
-        <v>-17.328099999999999</v>
+        <v>-12.6579</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
-        <v>18.22208703359744</v>
+        <f t="shared" si="1"/>
+        <v>13.437993675396635</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -812,18 +824,18 @@
         <v>-5.9726999999999997</v>
       </c>
       <c r="D19">
-        <f>SQRT((B19)^2+(C19)^2)</f>
+        <f t="shared" si="0"/>
         <v>6.1174079952215052</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1.2270000000000001</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>-6.3997000000000002</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>6.5162634300648099</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -837,18 +849,18 @@
         <v>-6.0347999999999997</v>
       </c>
       <c r="D20">
-        <f>SQRT((B20)^2+(C20)^2)</f>
+        <f t="shared" si="0"/>
         <v>6.0725214433544821</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.53620000000000001</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>-6.4583000000000004</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>6.4805207607105162</v>
       </c>
     </row>
   </sheetData>
@@ -858,10 +870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P7"/>
+  <dimension ref="A2:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:L7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,6 +953,26 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
+      <c r="B6">
+        <v>-46.525599999999997</v>
+      </c>
+      <c r="C6">
+        <v>-13.553699999999999</v>
+      </c>
+      <c r="D6">
+        <f>SQRT((B6)^2+(C6)^2)</f>
+        <v>48.459614516110214</v>
+      </c>
+      <c r="F6">
+        <v>-56.765700000000002</v>
+      </c>
+      <c r="G6">
+        <v>25.816299999999998</v>
+      </c>
+      <c r="H6">
+        <f>SQRT((F6)^2+(G6)^2)</f>
+        <v>62.360452549512502</v>
+      </c>
       <c r="J6">
         <v>17.800599999999999</v>
       </c>
@@ -966,15 +998,35 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
+      <c r="B7">
+        <v>-18.116700000000002</v>
+      </c>
+      <c r="C7">
+        <v>-5.7504</v>
+      </c>
+      <c r="D7">
+        <f>SQRT((B7)^2+(C7)^2)</f>
+        <v>19.007417474501896</v>
+      </c>
+      <c r="F7">
+        <v>-19.6312</v>
+      </c>
+      <c r="G7">
+        <v>0.14019999999999999</v>
+      </c>
+      <c r="H7">
+        <f>SQRT((F7)^2+(G7)^2)</f>
+        <v>19.631700626282992</v>
+      </c>
       <c r="J7">
-        <v>4.2830000000000004</v>
+        <v>3.9594999999999998</v>
       </c>
       <c r="K7">
-        <v>-15.3537</v>
+        <v>-13.8637</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>15.939893120407049</v>
+        <v>14.418037936557109</v>
       </c>
       <c r="N7">
         <v>6.64</v>
@@ -985,6 +1037,83 @@
       <c r="P7">
         <f>SQRT((N7)^2+(O7)^2)</f>
         <v>21.947817943704564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>22.4</v>
+      </c>
+      <c r="C11">
+        <v>-74.435500000000005</v>
+      </c>
+      <c r="D11">
+        <v>22.4</v>
+      </c>
+      <c r="E11">
+        <v>-74.435500000000005</v>
+      </c>
+      <c r="F11">
+        <v>22.4</v>
+      </c>
+      <c r="G11">
+        <v>-74.435500000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>5.2195299999999998</v>
+      </c>
+      <c r="C12">
+        <v>-74.442599999999999</v>
+      </c>
+      <c r="D12">
+        <v>5.2195299999999998</v>
+      </c>
+      <c r="E12">
+        <v>-74.442599999999999</v>
+      </c>
+      <c r="F12">
+        <v>5.2195299999999998</v>
+      </c>
+      <c r="G12">
+        <v>-74.442599999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
part B number 1 complete
</commit_message>
<xml_diff>
--- a/Fault Calcs.xlsx
+++ b/Fault Calcs.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\EE457\ee457project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\EE 457\ee457project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Part A" sheetId="1" r:id="rId1"/>
     <sheet name="Part B" sheetId="2" r:id="rId2"/>
+    <sheet name="Part 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t>Bus Num</t>
   </si>
@@ -145,6 +146,30 @@
   </si>
   <si>
     <t>Siskin out</t>
+  </si>
+  <si>
+    <t>Impedance</t>
+  </si>
+  <si>
+    <t>Phase a</t>
+  </si>
+  <si>
+    <t>Phase c</t>
+  </si>
+  <si>
+    <t>Rural Bus 11</t>
+  </si>
+  <si>
+    <t>Phase b</t>
+  </si>
+  <si>
+    <t>Zone 1</t>
+  </si>
+  <si>
+    <t>Zone 2</t>
+  </si>
+  <si>
+    <t>Zone 3</t>
   </si>
 </sst>
 </file>
@@ -465,7 +490,7 @@
   <dimension ref="A2:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,7 +960,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -1430,4 +1455,196 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" t="s">
+        <v>11</v>
+      </c>
+      <c r="P4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" t="s">
+        <v>12</v>
+      </c>
+      <c r="V4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W4" t="s">
+        <v>11</v>
+      </c>
+      <c r="X4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1.83E-2</v>
+      </c>
+      <c r="C5">
+        <v>0.1033</v>
+      </c>
+      <c r="D5">
+        <f>SQRT((B5)^2+(C5)^2)</f>
+        <v>0.10490843626706101</v>
+      </c>
+      <c r="F5">
+        <v>1.37E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.16769999999999999</v>
+      </c>
+      <c r="H5">
+        <f>SQRT((F5)^2+(G5)^2)</f>
+        <v>0.16825866991034963</v>
+      </c>
+      <c r="J5">
+        <v>-0.77159999999999995</v>
+      </c>
+      <c r="K5">
+        <v>0.41239999999999999</v>
+      </c>
+      <c r="L5">
+        <f>SQRT((J5)^2+(K5)^2)</f>
+        <v>0.87489446220672806</v>
+      </c>
+      <c r="N5">
+        <v>-0.71599999999999997</v>
+      </c>
+      <c r="O5">
+        <v>0.38179999999999997</v>
+      </c>
+      <c r="P5">
+        <f>SQRT((N5)^2+(O5)^2)</f>
+        <v>0.8114352962497996</v>
+      </c>
+      <c r="R5">
+        <v>-0.77159999999999995</v>
+      </c>
+      <c r="S5">
+        <v>0.41239999999999999</v>
+      </c>
+      <c r="T5">
+        <f>SQRT((R5)^2+(S5)^2)</f>
+        <v>0.87489446220672806</v>
+      </c>
+      <c r="V5">
+        <v>-0.71599999999999997</v>
+      </c>
+      <c r="W5">
+        <v>0.38179999999999997</v>
+      </c>
+      <c r="X5">
+        <f>SQRT((V5)^2+(W5)^2)</f>
+        <v>0.8114352962497996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>